<commit_message>
Return home functionality and calculation part checked
</commit_message>
<xml_diff>
--- a/Demo Excel.xlsx
+++ b/Demo Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Detector Software\V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Developed softwares\Detector Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBF81B9-BF87-4852-9881-17FF08F8E09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAA35B-4F8D-434C-BDAC-C3788F6224BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,10 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -257,7 +255,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384091A7-1262-415C-A5A0-F9559809C47E}">
   <dimension ref="A1:K139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,42 +585,42 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
@@ -633,10 +633,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
@@ -649,10 +649,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
@@ -665,10 +665,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
@@ -711,8 +711,8 @@
       <c r="G9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -729,8 +729,8 @@
       <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -749,10 +749,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
@@ -781,10 +781,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
@@ -797,10 +797,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,14 +813,14 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2532,32 +2532,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
@@ -2565,6 +2539,32 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>